<commit_message>
Etapa 5 refatoracao e melhoria completa
</commit_message>
<xml_diff>
--- a/output/relatorio_2025-12-26.xlsx
+++ b/output/relatorio_2025-12-26.xlsx
@@ -8,7 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="Resumo" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Detalhado" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Por Produto" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Por Dia" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Detalhado" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,11 +19,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-    <numFmt numFmtId="166" formatCode="R$ #,##0.00"/>
-    <numFmt numFmtId="167" formatCode="YYYY-MM-DD"/>
+  <numFmts count="6">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="168" formatCode="R$ #,##0.00"/>
+    <numFmt numFmtId="169" formatCode="0.00&quot;%&quot;"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -61,13 +65,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -143,6 +148,260 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Top 10 Produtos por Faturamento</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Por Produto'!B1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Por Produto'!$A$2:$A$10</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Por Produto'!$B$2:$B$10</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Faturamento (R$)</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Faturamento por Dia</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Por Dia'!B1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Por Dia'!$A$2:$A$98</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Por Dia'!$B$2:$B$98</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Faturamento (R$)</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="7200000" cy="3600000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="7200000" cy="3600000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -434,7 +693,152 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="26" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Métrica</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Valor</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Data de geração</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-12-26</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Período (início)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2024-10-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Período (fim)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-03-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Número de vendas</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Quantidade total</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Faturamento total</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>683177.6799999999</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Ticket médio</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>4554.517866666666</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Produto campeão</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Notebook</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Dia recorde</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2025-01-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Faturamento dia recorde</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>39833.06</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,69 +847,963 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="22" customWidth="1" min="1" max="1"/>
-    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="16" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Métrica</t>
+          <t>produto</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>faturamento</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>participacao_%</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Faturamento total</t>
+          <t>Notebook</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>683177.6799999999</v>
+        <v>315409.89</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>46.17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Quantidade total</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="n">
-        <v>864</v>
+          <t>Monitor</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>166653.56</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>24.39</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Produto campeão</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Notebook</t>
-        </is>
+          <t>Impressora</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>79778.3</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>11.68</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ticket médio</t>
+          <t>HD</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>4554.517866666666</v>
+        <v>35820.02</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>5.24</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SSD</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>32685.53</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>4.78</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Headset</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>19205.43</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>2.81</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Teclado</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>13517.13</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Webcam</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>12027.19</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Mouse</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>8080.63</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>1.18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B98"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>data</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>faturamento</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n">
+        <v>45570</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>4972.04</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="n">
+        <v>45571</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>753.78</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="n">
+        <v>45572</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>732.51</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n">
+        <v>45574</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>1468.9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n">
+        <v>45575</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>16421.02</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n">
+        <v>45576</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>958.72</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="n">
+        <v>45578</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>19641.65</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="n">
+        <v>45580</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>19480.9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="n">
+        <v>45581</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>7854.4</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="n">
+        <v>45583</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>12900.12</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="n">
+        <v>45588</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>23388.73</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="n">
+        <v>45592</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>16808.15</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="n">
+        <v>45594</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>25858.42</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="n">
+        <v>45596</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>1611.85</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="n">
+        <v>45597</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>6293.92</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="n">
+        <v>45598</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>14105.68</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="n">
+        <v>45600</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>4319.16</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="n">
+        <v>45603</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>1676.12</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="n">
+        <v>45608</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>6862.26</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="n">
+        <v>45609</v>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>5085.57</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="n">
+        <v>45610</v>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>3841.4</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="n">
+        <v>45611</v>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>2577.71</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="n">
+        <v>45613</v>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>1380.16</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="4" t="n">
+        <v>45615</v>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>6686.540000000001</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="n">
+        <v>45616</v>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>739.38</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="4" t="n">
+        <v>45620</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="4" t="n">
+        <v>45624</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>1198.39</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="4" t="n">
+        <v>45625</v>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>416.45</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="4" t="n">
+        <v>45628</v>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>31359.51</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="4" t="n">
+        <v>45631</v>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>2699.28</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="4" t="n">
+        <v>45633</v>
+      </c>
+      <c r="B32" s="2" t="n">
+        <v>14076.02</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="4" t="n">
+        <v>45635</v>
+      </c>
+      <c r="B33" s="2" t="n">
+        <v>620.38</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="4" t="n">
+        <v>45637</v>
+      </c>
+      <c r="B34" s="2" t="n">
+        <v>7149.66</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="4" t="n">
+        <v>45638</v>
+      </c>
+      <c r="B35" s="2" t="n">
+        <v>2390.62</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="4" t="n">
+        <v>45641</v>
+      </c>
+      <c r="B36" s="2" t="n">
+        <v>661.04</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="4" t="n">
+        <v>45644</v>
+      </c>
+      <c r="B37" s="2" t="n">
+        <v>3246.32</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="4" t="n">
+        <v>45645</v>
+      </c>
+      <c r="B38" s="2" t="n">
+        <v>924.8600000000001</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="4" t="n">
+        <v>45647</v>
+      </c>
+      <c r="B39" s="2" t="n">
+        <v>2699.37</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="4" t="n">
+        <v>45648</v>
+      </c>
+      <c r="B40" s="2" t="n">
+        <v>664.46</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="4" t="n">
+        <v>45649</v>
+      </c>
+      <c r="B41" s="2" t="n">
+        <v>7278.210000000001</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="4" t="n">
+        <v>45651</v>
+      </c>
+      <c r="B42" s="2" t="n">
+        <v>3599.01</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="4" t="n">
+        <v>45653</v>
+      </c>
+      <c r="B43" s="2" t="n">
+        <v>9953.92</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="4" t="n">
+        <v>45654</v>
+      </c>
+      <c r="B44" s="2" t="n">
+        <v>1186.56</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="4" t="n">
+        <v>45655</v>
+      </c>
+      <c r="B45" s="2" t="n">
+        <v>613.76</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="4" t="n">
+        <v>45658</v>
+      </c>
+      <c r="B46" s="2" t="n">
+        <v>21123.42</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="4" t="n">
+        <v>45659</v>
+      </c>
+      <c r="B47" s="2" t="n">
+        <v>472.42</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="4" t="n">
+        <v>45664</v>
+      </c>
+      <c r="B48" s="2" t="n">
+        <v>10910.88</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="4" t="n">
+        <v>45665</v>
+      </c>
+      <c r="B49" s="2" t="n">
+        <v>4874.18</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="4" t="n">
+        <v>45667</v>
+      </c>
+      <c r="B50" s="2" t="n">
+        <v>8076.879999999999</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="4" t="n">
+        <v>45668</v>
+      </c>
+      <c r="B51" s="2" t="n">
+        <v>5124.21</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="4" t="n">
+        <v>45670</v>
+      </c>
+      <c r="B52" s="2" t="n">
+        <v>11060.73</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="4" t="n">
+        <v>45671</v>
+      </c>
+      <c r="B53" s="2" t="n">
+        <v>908.15</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="4" t="n">
+        <v>45673</v>
+      </c>
+      <c r="B54" s="2" t="n">
+        <v>16948.28</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="4" t="n">
+        <v>45676</v>
+      </c>
+      <c r="B55" s="2" t="n">
+        <v>1559.44</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="4" t="n">
+        <v>45677</v>
+      </c>
+      <c r="B56" s="2" t="n">
+        <v>1880.16</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="4" t="n">
+        <v>45678</v>
+      </c>
+      <c r="B57" s="2" t="n">
+        <v>4393.83</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="4" t="n">
+        <v>45679</v>
+      </c>
+      <c r="B58" s="2" t="n">
+        <v>39833.06</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="4" t="n">
+        <v>45680</v>
+      </c>
+      <c r="B59" s="2" t="n">
+        <v>1205.32</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="4" t="n">
+        <v>45681</v>
+      </c>
+      <c r="B60" s="2" t="n">
+        <v>1280.02</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="4" t="n">
+        <v>45684</v>
+      </c>
+      <c r="B61" s="2" t="n">
+        <v>381.4</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="4" t="n">
+        <v>45685</v>
+      </c>
+      <c r="B62" s="2" t="n">
+        <v>1311.54</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="4" t="n">
+        <v>45686</v>
+      </c>
+      <c r="B63" s="2" t="n">
+        <v>28890.56</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="4" t="n">
+        <v>45688</v>
+      </c>
+      <c r="B64" s="2" t="n">
+        <v>1964.05</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="4" t="n">
+        <v>45689</v>
+      </c>
+      <c r="B65" s="2" t="n">
+        <v>3736.56</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="4" t="n">
+        <v>45691</v>
+      </c>
+      <c r="B66" s="2" t="n">
+        <v>1300.79</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="4" t="n">
+        <v>45692</v>
+      </c>
+      <c r="B67" s="2" t="n">
+        <v>27488.72</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="4" t="n">
+        <v>45693</v>
+      </c>
+      <c r="B68" s="2" t="n">
+        <v>1394.28</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="4" t="n">
+        <v>45694</v>
+      </c>
+      <c r="B69" s="2" t="n">
+        <v>307.48</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="4" t="n">
+        <v>45695</v>
+      </c>
+      <c r="B70" s="2" t="n">
+        <v>1497.5</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="4" t="n">
+        <v>45696</v>
+      </c>
+      <c r="B71" s="2" t="n">
+        <v>236.37</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="4" t="n">
+        <v>45700</v>
+      </c>
+      <c r="B72" s="2" t="n">
+        <v>17002.3</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="4" t="n">
+        <v>45701</v>
+      </c>
+      <c r="B73" s="2" t="n">
+        <v>6181.549999999999</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="4" t="n">
+        <v>45705</v>
+      </c>
+      <c r="B74" s="2" t="n">
+        <v>2524.7</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="4" t="n">
+        <v>45708</v>
+      </c>
+      <c r="B75" s="2" t="n">
+        <v>8439.290000000001</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="4" t="n">
+        <v>45710</v>
+      </c>
+      <c r="B76" s="2" t="n">
+        <v>6273.04</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="4" t="n">
+        <v>45711</v>
+      </c>
+      <c r="B77" s="2" t="n">
+        <v>5166.53</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="4" t="n">
+        <v>45712</v>
+      </c>
+      <c r="B78" s="2" t="n">
+        <v>1358.58</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="4" t="n">
+        <v>45715</v>
+      </c>
+      <c r="B79" s="2" t="n">
+        <v>13738.06</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="4" t="n">
+        <v>45716</v>
+      </c>
+      <c r="B80" s="2" t="n">
+        <v>3805.3</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="4" t="n">
+        <v>45718</v>
+      </c>
+      <c r="B81" s="2" t="n">
+        <v>11512.94</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="4" t="n">
+        <v>45720</v>
+      </c>
+      <c r="B82" s="2" t="n">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="4" t="n">
+        <v>45722</v>
+      </c>
+      <c r="B83" s="2" t="n">
+        <v>1801.41</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="4" t="n">
+        <v>45723</v>
+      </c>
+      <c r="B84" s="2" t="n">
+        <v>785.95</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="4" t="n">
+        <v>45725</v>
+      </c>
+      <c r="B85" s="2" t="n">
+        <v>5604.69</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="4" t="n">
+        <v>45726</v>
+      </c>
+      <c r="B86" s="2" t="n">
+        <v>15940.64</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="4" t="n">
+        <v>45727</v>
+      </c>
+      <c r="B87" s="2" t="n">
+        <v>11535.4</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="4" t="n">
+        <v>45728</v>
+      </c>
+      <c r="B88" s="2" t="n">
+        <v>1087.86</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="4" t="n">
+        <v>45730</v>
+      </c>
+      <c r="B89" s="2" t="n">
+        <v>731.8799999999999</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="4" t="n">
+        <v>45731</v>
+      </c>
+      <c r="B90" s="2" t="n">
+        <v>3475.98</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="4" t="n">
+        <v>45733</v>
+      </c>
+      <c r="B91" s="2" t="n">
+        <v>1766.46</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="4" t="n">
+        <v>45735</v>
+      </c>
+      <c r="B92" s="2" t="n">
+        <v>4036.8</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="4" t="n">
+        <v>45737</v>
+      </c>
+      <c r="B93" s="2" t="n">
+        <v>1246.15</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="4" t="n">
+        <v>45738</v>
+      </c>
+      <c r="B94" s="2" t="n">
+        <v>1077.37</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="4" t="n">
+        <v>45739</v>
+      </c>
+      <c r="B95" s="2" t="n">
+        <v>22924.76</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="4" t="n">
+        <v>45743</v>
+      </c>
+      <c r="B96" s="2" t="n">
+        <v>27868.3</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="4" t="n">
+        <v>45744</v>
+      </c>
+      <c r="B97" s="2" t="n">
+        <v>7633.7</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="4" t="n">
+        <v>45746</v>
+      </c>
+      <c r="B98" s="2" t="n">
+        <v>2786.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -518,13 +1816,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="14" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="16" customWidth="1" min="4" max="4"/>
-    <col width="16" customWidth="1" min="5" max="5"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -554,7 +1845,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="n">
+      <c r="A2" s="5" t="n">
         <v>45570</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -562,7 +1853,7 @@
           <t>Monitor</t>
         </is>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" t="n">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="n">
@@ -573,7 +1864,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="n">
+      <c r="A3" s="5" t="n">
         <v>45571</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -581,7 +1872,7 @@
           <t>Headset</t>
         </is>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" t="n">
         <v>3</v>
       </c>
       <c r="D3" s="2" t="n">
@@ -592,7 +1883,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="n">
+      <c r="A4" s="5" t="n">
         <v>45572</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -600,7 +1891,7 @@
           <t>Mouse</t>
         </is>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" t="n">
         <v>9</v>
       </c>
       <c r="D4" s="2" t="n">
@@ -611,7 +1902,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="n">
+      <c r="A5" s="5" t="n">
         <v>45574</v>
       </c>
       <c r="B5" t="inlineStr">
@@ -619,7 +1910,7 @@
           <t>HD</t>
         </is>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" t="n">
         <v>5</v>
       </c>
       <c r="D5" s="2" t="n">
@@ -630,7 +1921,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="n">
+      <c r="A6" s="5" t="n">
         <v>45575</v>
       </c>
       <c r="B6" t="inlineStr">
@@ -638,7 +1929,7 @@
           <t>Impressora</t>
         </is>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" t="n">
         <v>9</v>
       </c>
       <c r="D6" s="2" t="n">
@@ -649,7 +1940,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="n">
+      <c r="A7" s="5" t="n">
         <v>45575</v>
       </c>
       <c r="B7" t="inlineStr">
@@ -657,7 +1948,7 @@
           <t>Monitor</t>
         </is>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" t="n">
         <v>8</v>
       </c>
       <c r="D7" s="2" t="n">
@@ -668,7 +1959,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="n">
+      <c r="A8" s="5" t="n">
         <v>45576</v>
       </c>
       <c r="B8" t="inlineStr">
@@ -676,7 +1967,7 @@
           <t>Headset</t>
         </is>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" t="n">
         <v>4</v>
       </c>
       <c r="D8" s="2" t="n">
@@ -687,7 +1978,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="n">
+      <c r="A9" s="5" t="n">
         <v>45578</v>
       </c>
       <c r="B9" t="inlineStr">
@@ -695,7 +1986,7 @@
           <t>Notebook</t>
         </is>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C9" t="n">
         <v>5</v>
       </c>
       <c r="D9" s="2" t="n">
@@ -706,7 +1997,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="n">
+      <c r="A10" s="5" t="n">
         <v>45578</v>
       </c>
       <c r="B10" t="inlineStr">
@@ -714,7 +2005,7 @@
           <t>HD</t>
         </is>
       </c>
-      <c r="C10" s="3" t="n">
+      <c r="C10" t="n">
         <v>10</v>
       </c>
       <c r="D10" s="2" t="n">
@@ -725,7 +2016,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="n">
+      <c r="A11" s="5" t="n">
         <v>45580</v>
       </c>
       <c r="B11" t="inlineStr">
@@ -733,7 +2024,7 @@
           <t>Monitor</t>
         </is>
       </c>
-      <c r="C11" s="3" t="n">
+      <c r="C11" t="n">
         <v>10</v>
       </c>
       <c r="D11" s="2" t="n">
@@ -744,7 +2035,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="n">
+      <c r="A12" s="5" t="n">
         <v>45580</v>
       </c>
       <c r="B12" t="inlineStr">
@@ -752,7 +2043,7 @@
           <t>Impressora</t>
         </is>
       </c>
-      <c r="C12" s="3" t="n">
+      <c r="C12" t="n">
         <v>10</v>
       </c>
       <c r="D12" s="2" t="n">
@@ -763,7 +2054,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="n">
+      <c r="A13" s="5" t="n">
         <v>45581</v>
       </c>
       <c r="B13" t="inlineStr">
@@ -771,7 +2062,7 @@
           <t>Teclado</t>
         </is>
       </c>
-      <c r="C13" s="3" t="n">
+      <c r="C13" t="n">
         <v>8</v>
       </c>
       <c r="D13" s="2" t="n">
@@ -782,7 +2073,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="n">
+      <c r="A14" s="5" t="n">
         <v>45581</v>
       </c>
       <c r="B14" t="inlineStr">
@@ -790,7 +2081,7 @@
           <t>Impressora</t>
         </is>
       </c>
-      <c r="C14" s="3" t="n">
+      <c r="C14" t="n">
         <v>8</v>
       </c>
       <c r="D14" s="2" t="n">
@@ -801,7 +2092,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="4" t="n">
+      <c r="A15" s="5" t="n">
         <v>45583</v>
       </c>
       <c r="B15" t="inlineStr">
@@ -809,7 +2100,7 @@
           <t>SSD</t>
         </is>
       </c>
-      <c r="C15" s="3" t="n">
+      <c r="C15" t="n">
         <v>6</v>
       </c>
       <c r="D15" s="2" t="n">
@@ -820,7 +2111,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="n">
+      <c r="A16" s="5" t="n">
         <v>45583</v>
       </c>
       <c r="B16" t="inlineStr">
@@ -828,7 +2119,7 @@
           <t>Monitor</t>
         </is>
       </c>
-      <c r="C16" s="3" t="n">
+      <c r="C16" t="n">
         <v>9</v>
       </c>
       <c r="D16" s="2" t="n">
@@ -839,7 +2130,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="n">
+      <c r="A17" s="5" t="n">
         <v>45588</v>
       </c>
       <c r="B17" t="inlineStr">
@@ -847,7 +2138,7 @@
           <t>Webcam</t>
         </is>
       </c>
-      <c r="C17" s="3" t="n">
+      <c r="C17" t="n">
         <v>7</v>
       </c>
       <c r="D17" s="2" t="n">
@@ -858,7 +2149,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="n">
+      <c r="A18" s="5" t="n">
         <v>45588</v>
       </c>
       <c r="B18" t="inlineStr">
@@ -866,7 +2157,7 @@
           <t>Mouse</t>
         </is>
       </c>
-      <c r="C18" s="3" t="n">
+      <c r="C18" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="2" t="n">
@@ -877,7 +2168,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="4" t="n">
+      <c r="A19" s="5" t="n">
         <v>45588</v>
       </c>
       <c r="B19" t="inlineStr">
@@ -885,7 +2176,7 @@
           <t>Mouse</t>
         </is>
       </c>
-      <c r="C19" s="3" t="n">
+      <c r="C19" t="n">
         <v>5</v>
       </c>
       <c r="D19" s="2" t="n">
@@ -896,7 +2187,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="4" t="n">
+      <c r="A20" s="5" t="n">
         <v>45588</v>
       </c>
       <c r="B20" t="inlineStr">
@@ -904,7 +2195,7 @@
           <t>Notebook</t>
         </is>
       </c>
-      <c r="C20" s="3" t="n">
+      <c r="C20" t="n">
         <v>6</v>
       </c>
       <c r="D20" s="2" t="n">
@@ -915,7 +2206,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="4" t="n">
+      <c r="A21" s="5" t="n">
         <v>45592</v>
       </c>
       <c r="B21" t="inlineStr">
@@ -923,7 +2214,7 @@
           <t>Notebook</t>
         </is>
       </c>
-      <c r="C21" s="3" t="n">
+      <c r="C21" t="n">
         <v>5</v>
       </c>
       <c r="D21" s="2" t="n">
@@ -934,7 +2225,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="4" t="n">
+      <c r="A22" s="5" t="n">
         <v>45594</v>
       </c>
       <c r="B22" t="inlineStr">
@@ -942,7 +2233,7 @@
           <t>Notebook</t>
         </is>
       </c>
-      <c r="C22" s="3" t="n">
+      <c r="C22" t="n">
         <v>7</v>
       </c>
       <c r="D22" s="2" t="n">
@@ -953,7 +2244,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="4" t="n">
+      <c r="A23" s="5" t="n">
         <v>45594</v>
       </c>
       <c r="B23" t="inlineStr">
@@ -961,7 +2252,7 @@
           <t>HD</t>
         </is>
       </c>
-      <c r="C23" s="3" t="n">
+      <c r="C23" t="n">
         <v>6</v>
       </c>
       <c r="D23" s="2" t="n">
@@ -972,7 +2263,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="4" t="n">
+      <c r="A24" s="5" t="n">
         <v>45596</v>
       </c>
       <c r="B24" t="inlineStr">
@@ -980,7 +2271,7 @@
           <t>Teclado</t>
         </is>
       </c>
-      <c r="C24" s="3" t="n">
+      <c r="C24" t="n">
         <v>5</v>
       </c>
       <c r="D24" s="2" t="n">
@@ -991,7 +2282,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="n">
+      <c r="A25" s="5" t="n">
         <v>45596</v>
       </c>
       <c r="B25" t="inlineStr">
@@ -999,7 +2290,7 @@
           <t>Webcam</t>
         </is>
       </c>
-      <c r="C25" s="3" t="n">
+      <c r="C25" t="n">
         <v>5</v>
       </c>
       <c r="D25" s="2" t="n">
@@ -1010,7 +2301,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="4" t="n">
+      <c r="A26" s="5" t="n">
         <v>45597</v>
       </c>
       <c r="B26" t="inlineStr">
@@ -1018,7 +2309,7 @@
           <t>Impressora</t>
         </is>
       </c>
-      <c r="C26" s="3" t="n">
+      <c r="C26" t="n">
         <v>8</v>
       </c>
       <c r="D26" s="2" t="n">
@@ -1029,7 +2320,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="4" t="n">
+      <c r="A27" s="5" t="n">
         <v>45598</v>
       </c>
       <c r="B27" t="inlineStr">
@@ -1037,7 +2328,7 @@
           <t>Notebook</t>
         </is>
       </c>
-      <c r="C27" s="3" t="n">
+      <c r="C27" t="n">
         <v>4</v>
       </c>
       <c r="D27" s="2" t="n">
@@ -1048,7 +2339,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="4" t="n">
+      <c r="A28" s="5" t="n">
         <v>45600</v>
       </c>
       <c r="B28" t="inlineStr">
@@ -1056,7 +2347,7 @@
           <t>HD</t>
         </is>
       </c>
-      <c r="C28" s="3" t="n">
+      <c r="C28" t="n">
         <v>9</v>
       </c>
       <c r="D28" s="2" t="n">
@@ -1067,7 +2358,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="4" t="n">
+      <c r="A29" s="5" t="n">
         <v>45600</v>
       </c>
       <c r="B29" t="inlineStr">
@@ -1075,7 +2366,7 @@
           <t>SSD</t>
         </is>
       </c>
-      <c r="C29" s="3" t="n">
+      <c r="C29" t="n">
         <v>4</v>
       </c>
       <c r="D29" s="2" t="n">
@@ -1086,7 +2377,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="4" t="n">
+      <c r="A30" s="5" t="n">
         <v>45603</v>
       </c>
       <c r="B30" t="inlineStr">
@@ -1094,7 +2385,7 @@
           <t>Impressora</t>
         </is>
       </c>
-      <c r="C30" s="3" t="n">
+      <c r="C30" t="n">
         <v>2</v>
       </c>
       <c r="D30" s="2" t="n">
@@ -1105,7 +2396,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="4" t="n">
+      <c r="A31" s="5" t="n">
         <v>45608</v>
       </c>
       <c r="B31" t="inlineStr">
@@ -1113,7 +2404,7 @@
           <t>Notebook</t>
         </is>
       </c>
-      <c r="C31" s="3" t="n">
+      <c r="C31" t="n">
         <v>2</v>
       </c>
       <c r="D31" s="2" t="n">
@@ -1124,7 +2415,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="4" t="n">
+      <c r="A32" s="5" t="n">
         <v>45609</v>
       </c>
       <c r="B32" t="inlineStr">
@@ -1132,7 +2423,7 @@
           <t>SSD</t>
         </is>
       </c>
-      <c r="C32" s="3" t="n">
+      <c r="C32" t="n">
         <v>6</v>
       </c>
       <c r="D32" s="2" t="n">
@@ -1143,7 +2434,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="4" t="n">
+      <c r="A33" s="5" t="n">
         <v>45609</v>
       </c>
       <c r="B33" t="inlineStr">
@@ -1151,7 +2442,7 @@
           <t>HD</t>
         </is>
       </c>
-      <c r="C33" s="3" t="n">
+      <c r="C33" t="n">
         <v>9</v>
       </c>
       <c r="D33" s="2" t="n">
@@ -1162,7 +2453,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="4" t="n">
+      <c r="A34" s="5" t="n">
         <v>45610</v>
       </c>
       <c r="B34" t="inlineStr">
@@ -1170,7 +2461,7 @@
           <t>HD</t>
         </is>
       </c>
-      <c r="C34" s="3" t="n">
+      <c r="C34" t="n">
         <v>10</v>
       </c>
       <c r="D34" s="2" t="n">
@@ -1181,7 +2472,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="4" t="n">
+      <c r="A35" s="5" t="n">
         <v>45610</v>
       </c>
       <c r="B35" t="inlineStr">
@@ -1189,7 +2480,7 @@
           <t>Webcam</t>
         </is>
       </c>
-      <c r="C35" s="3" t="n">
+      <c r="C35" t="n">
         <v>5</v>
       </c>
       <c r="D35" s="2" t="n">
@@ -1200,7 +2491,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="4" t="n">
+      <c r="A36" s="5" t="n">
         <v>45611</v>
       </c>
       <c r="B36" t="inlineStr">
@@ -1208,7 +2499,7 @@
           <t>Monitor</t>
         </is>
       </c>
-      <c r="C36" s="3" t="n">
+      <c r="C36" t="n">
         <v>1</v>
       </c>
       <c r="D36" s="2" t="n">
@@ -1219,7 +2510,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="4" t="n">
+      <c r="A37" s="5" t="n">
         <v>45611</v>
       </c>
       <c r="B37" t="inlineStr">
@@ -1227,7 +2518,7 @@
           <t>Teclado</t>
         </is>
       </c>
-      <c r="C37" s="3" t="n">
+      <c r="C37" t="n">
         <v>9</v>
       </c>
       <c r="D37" s="2" t="n">
@@ -1238,7 +2529,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="4" t="n">
+      <c r="A38" s="5" t="n">
         <v>45613</v>
       </c>
       <c r="B38" t="inlineStr">
@@ -1246,7 +2537,7 @@
           <t>Webcam</t>
         </is>
       </c>
-      <c r="C38" s="3" t="n">
+      <c r="C38" t="n">
         <v>8</v>
       </c>
       <c r="D38" s="2" t="n">
@@ -1257,7 +2548,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="4" t="n">
+      <c r="A39" s="5" t="n">
         <v>45615</v>
       </c>
       <c r="B39" t="inlineStr">
@@ -1265,7 +2556,7 @@
           <t>Impressora</t>
         </is>
       </c>
-      <c r="C39" s="3" t="n">
+      <c r="C39" t="n">
         <v>7</v>
       </c>
       <c r="D39" s="2" t="n">
@@ -1276,7 +2567,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="4" t="n">
+      <c r="A40" s="5" t="n">
         <v>45615</v>
       </c>
       <c r="B40" t="inlineStr">
@@ -1284,7 +2575,7 @@
           <t>Teclado</t>
         </is>
       </c>
-      <c r="C40" s="3" t="n">
+      <c r="C40" t="n">
         <v>8</v>
       </c>
       <c r="D40" s="2" t="n">
@@ -1295,7 +2586,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="4" t="n">
+      <c r="A41" s="5" t="n">
         <v>45616</v>
       </c>
       <c r="B41" t="inlineStr">
@@ -1303,7 +2594,7 @@
           <t>Headset</t>
         </is>
       </c>
-      <c r="C41" s="3" t="n">
+      <c r="C41" t="n">
         <v>3</v>
       </c>
       <c r="D41" s="2" t="n">
@@ -1314,7 +2605,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="4" t="n">
+      <c r="A42" s="5" t="n">
         <v>45620</v>
       </c>
       <c r="B42" t="inlineStr">
@@ -1322,7 +2613,7 @@
           <t>Teclado</t>
         </is>
       </c>
-      <c r="C42" s="3" t="n">
+      <c r="C42" t="n">
         <v>3</v>
       </c>
       <c r="D42" s="2" t="n">
@@ -1333,7 +2624,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="4" t="n">
+      <c r="A43" s="5" t="n">
         <v>45620</v>
       </c>
       <c r="B43" t="inlineStr">
@@ -1341,7 +2632,7 @@
           <t>Webcam</t>
         </is>
       </c>
-      <c r="C43" s="3" t="n">
+      <c r="C43" t="n">
         <v>1</v>
       </c>
       <c r="D43" s="2" t="n">
@@ -1352,7 +2643,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="4" t="n">
+      <c r="A44" s="5" t="n">
         <v>45624</v>
       </c>
       <c r="B44" t="inlineStr">
@@ -1360,7 +2651,7 @@
           <t>Monitor</t>
         </is>
       </c>
-      <c r="C44" s="3" t="n">
+      <c r="C44" t="n">
         <v>1</v>
       </c>
       <c r="D44" s="2" t="n">
@@ -1371,7 +2662,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="4" t="n">
+      <c r="A45" s="5" t="n">
         <v>45625</v>
       </c>
       <c r="B45" t="inlineStr">
@@ -1379,7 +2670,7 @@
           <t>Mouse</t>
         </is>
       </c>
-      <c r="C45" s="3" t="n">
+      <c r="C45" t="n">
         <v>5</v>
       </c>
       <c r="D45" s="2" t="n">
@@ -1390,7 +2681,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="4" t="n">
+      <c r="A46" s="5" t="n">
         <v>45628</v>
       </c>
       <c r="B46" t="inlineStr">
@@ -1398,7 +2689,7 @@
           <t>Notebook</t>
         </is>
       </c>
-      <c r="C46" s="3" t="n">
+      <c r="C46" t="n">
         <v>9</v>
       </c>
       <c r="D46" s="2" t="n">
@@ -1409,7 +2700,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="4" t="n">
+      <c r="A47" s="5" t="n">
         <v>45631</v>
       </c>
       <c r="B47" t="inlineStr">
@@ -1417,7 +2708,7 @@
           <t>Webcam</t>
         </is>
       </c>
-      <c r="C47" s="3" t="n">
+      <c r="C47" t="n">
         <v>6</v>
       </c>
       <c r="D47" s="2" t="n">
@@ -1428,7 +2719,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="4" t="n">
+      <c r="A48" s="5" t="n">
         <v>45631</v>
       </c>
       <c r="B48" t="inlineStr">
@@ -1436,7 +2727,7 @@
           <t>SSD</t>
         </is>
       </c>
-      <c r="C48" s="3" t="n">
+      <c r="C48" t="n">
         <v>4</v>
       </c>
       <c r="D48" s="2" t="n">
@@ -1447,7 +2738,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="4" t="n">
+      <c r="A49" s="5" t="n">
         <v>45633</v>
       </c>
       <c r="B49" t="inlineStr">
@@ -1455,7 +2746,7 @@
           <t>SSD</t>
         </is>
       </c>
-      <c r="C49" s="3" t="n">
+      <c r="C49" t="n">
         <v>8</v>
       </c>
       <c r="D49" s="2" t="n">
@@ -1466,7 +2757,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="4" t="n">
+      <c r="A50" s="5" t="n">
         <v>45633</v>
       </c>
       <c r="B50" t="inlineStr">
@@ -1474,7 +2765,7 @@
           <t>Monitor</t>
         </is>
       </c>
-      <c r="C50" s="3" t="n">
+      <c r="C50" t="n">
         <v>8</v>
       </c>
       <c r="D50" s="2" t="n">
@@ -1485,7 +2776,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="4" t="n">
+      <c r="A51" s="5" t="n">
         <v>45633</v>
       </c>
       <c r="B51" t="inlineStr">
@@ -1493,7 +2784,7 @@
           <t>SSD</t>
         </is>
       </c>
-      <c r="C51" s="3" t="n">
+      <c r="C51" t="n">
         <v>2</v>
       </c>
       <c r="D51" s="2" t="n">
@@ -1504,7 +2795,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="4" t="n">
+      <c r="A52" s="5" t="n">
         <v>45635</v>
       </c>
       <c r="B52" t="inlineStr">
@@ -1512,7 +2803,7 @@
           <t>HD</t>
         </is>
       </c>
-      <c r="C52" s="3" t="n">
+      <c r="C52" t="n">
         <v>2</v>
       </c>
       <c r="D52" s="2" t="n">
@@ -1523,7 +2814,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="4" t="n">
+      <c r="A53" s="5" t="n">
         <v>45637</v>
       </c>
       <c r="B53" t="inlineStr">
@@ -1531,7 +2822,7 @@
           <t>Impressora</t>
         </is>
       </c>
-      <c r="C53" s="3" t="n">
+      <c r="C53" t="n">
         <v>4</v>
       </c>
       <c r="D53" s="2" t="n">
@@ -1542,7 +2833,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="4" t="n">
+      <c r="A54" s="5" t="n">
         <v>45637</v>
       </c>
       <c r="B54" t="inlineStr">
@@ -1550,7 +2841,7 @@
           <t>Impressora</t>
         </is>
       </c>
-      <c r="C54" s="3" t="n">
+      <c r="C54" t="n">
         <v>5</v>
       </c>
       <c r="D54" s="2" t="n">
@@ -1561,7 +2852,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="4" t="n">
+      <c r="A55" s="5" t="n">
         <v>45638</v>
       </c>
       <c r="B55" t="inlineStr">
@@ -1569,7 +2860,7 @@
           <t>Monitor</t>
         </is>
       </c>
-      <c r="C55" s="3" t="n">
+      <c r="C55" t="n">
         <v>2</v>
       </c>
       <c r="D55" s="2" t="n">
@@ -1580,7 +2871,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="4" t="n">
+      <c r="A56" s="5" t="n">
         <v>45641</v>
       </c>
       <c r="B56" t="inlineStr">
@@ -1588,7 +2879,7 @@
           <t>Mouse</t>
         </is>
       </c>
-      <c r="C56" s="3" t="n">
+      <c r="C56" t="n">
         <v>8</v>
       </c>
       <c r="D56" s="2" t="n">
@@ -1599,7 +2890,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="4" t="n">
+      <c r="A57" s="5" t="n">
         <v>45644</v>
       </c>
       <c r="B57" t="inlineStr">
@@ -1607,7 +2898,7 @@
           <t>Headset</t>
         </is>
       </c>
-      <c r="C57" s="3" t="n">
+      <c r="C57" t="n">
         <v>4</v>
       </c>
       <c r="D57" s="2" t="n">
@@ -1618,7 +2909,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="4" t="n">
+      <c r="A58" s="5" t="n">
         <v>45644</v>
       </c>
       <c r="B58" t="inlineStr">
@@ -1626,7 +2917,7 @@
           <t>Monitor</t>
         </is>
       </c>
-      <c r="C58" s="3" t="n">
+      <c r="C58" t="n">
         <v>2</v>
       </c>
       <c r="D58" s="2" t="n">
@@ -1637,7 +2928,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="4" t="n">
+      <c r="A59" s="5" t="n">
         <v>45645</v>
       </c>
       <c r="B59" t="inlineStr">
@@ -1645,7 +2936,7 @@
           <t>Teclado</t>
         </is>
       </c>
-      <c r="C59" s="3" t="n">
+      <c r="C59" t="n">
         <v>1</v>
       </c>
       <c r="D59" s="2" t="n">
@@ -1656,7 +2947,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="4" t="n">
+      <c r="A60" s="5" t="n">
         <v>45645</v>
       </c>
       <c r="B60" t="inlineStr">
@@ -1664,7 +2955,7 @@
           <t>Teclado</t>
         </is>
       </c>
-      <c r="C60" s="3" t="n">
+      <c r="C60" t="n">
         <v>5</v>
       </c>
       <c r="D60" s="2" t="n">
@@ -1675,7 +2966,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="4" t="n">
+      <c r="A61" s="5" t="n">
         <v>45647</v>
       </c>
       <c r="B61" t="inlineStr">
@@ -1683,7 +2974,7 @@
           <t>HD</t>
         </is>
       </c>
-      <c r="C61" s="3" t="n">
+      <c r="C61" t="n">
         <v>9</v>
       </c>
       <c r="D61" s="2" t="n">
@@ -1694,7 +2985,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="4" t="n">
+      <c r="A62" s="5" t="n">
         <v>45648</v>
       </c>
       <c r="B62" t="inlineStr">
@@ -1702,7 +2993,7 @@
           <t>Mouse</t>
         </is>
       </c>
-      <c r="C62" s="3" t="n">
+      <c r="C62" t="n">
         <v>6</v>
       </c>
       <c r="D62" s="2" t="n">
@@ -1713,7 +3004,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="4" t="n">
+      <c r="A63" s="5" t="n">
         <v>45648</v>
       </c>
       <c r="B63" t="inlineStr">
@@ -1721,7 +3012,7 @@
           <t>Mouse</t>
         </is>
       </c>
-      <c r="C63" s="3" t="n">
+      <c r="C63" t="n">
         <v>2</v>
       </c>
       <c r="D63" s="2" t="n">
@@ -1732,7 +3023,7 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="4" t="n">
+      <c r="A64" s="5" t="n">
         <v>45649</v>
       </c>
       <c r="B64" t="inlineStr">
@@ -1740,7 +3031,7 @@
           <t>Impressora</t>
         </is>
       </c>
-      <c r="C64" s="3" t="n">
+      <c r="C64" t="n">
         <v>9</v>
       </c>
       <c r="D64" s="2" t="n">
@@ -1751,7 +3042,7 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="4" t="n">
+      <c r="A65" s="5" t="n">
         <v>45651</v>
       </c>
       <c r="B65" t="inlineStr">
@@ -1759,7 +3050,7 @@
           <t>Monitor</t>
         </is>
       </c>
-      <c r="C65" s="3" t="n">
+      <c r="C65" t="n">
         <v>3</v>
       </c>
       <c r="D65" s="2" t="n">
@@ -1770,7 +3061,7 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="4" t="n">
+      <c r="A66" s="5" t="n">
         <v>45653</v>
       </c>
       <c r="B66" t="inlineStr">
@@ -1778,7 +3069,7 @@
           <t>Monitor</t>
         </is>
       </c>
-      <c r="C66" s="3" t="n">
+      <c r="C66" t="n">
         <v>8</v>
       </c>
       <c r="D66" s="2" t="n">
@@ -1789,7 +3080,7 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="4" t="n">
+      <c r="A67" s="5" t="n">
         <v>45654</v>
       </c>
       <c r="B67" t="inlineStr">
@@ -1797,7 +3088,7 @@
           <t>Monitor</t>
         </is>
       </c>
-      <c r="C67" s="3" t="n">
+      <c r="C67" t="n">
         <v>1</v>
       </c>
       <c r="D67" s="2" t="n">
@@ -1808,7 +3099,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="4" t="n">
+      <c r="A68" s="5" t="n">
         <v>45655</v>
       </c>
       <c r="B68" t="inlineStr">
@@ -1816,7 +3107,7 @@
           <t>Mouse</t>
         </is>
       </c>
-      <c r="C68" s="3" t="n">
+      <c r="C68" t="n">
         <v>8</v>
       </c>
       <c r="D68" s="2" t="n">
@@ -1827,7 +3118,7 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="4" t="n">
+      <c r="A69" s="5" t="n">
         <v>45658</v>
       </c>
       <c r="B69" t="inlineStr">
@@ -1835,7 +3126,7 @@
           <t>Notebook</t>
         </is>
       </c>
-      <c r="C69" s="3" t="n">
+      <c r="C69" t="n">
         <v>6</v>
       </c>
       <c r="D69" s="2" t="n">
@@ -1846,7 +3137,7 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="4" t="n">
+      <c r="A70" s="5" t="n">
         <v>45659</v>
       </c>
       <c r="B70" t="inlineStr">
@@ -1854,7 +3145,7 @@
           <t>SSD</t>
         </is>
       </c>
-      <c r="C70" s="3" t="n">
+      <c r="C70" t="n">
         <v>1</v>
       </c>
       <c r="D70" s="2" t="n">
@@ -1865,7 +3156,7 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="4" t="n">
+      <c r="A71" s="5" t="n">
         <v>45659</v>
       </c>
       <c r="B71" t="inlineStr">
@@ -1873,7 +3164,7 @@
           <t>Mouse</t>
         </is>
       </c>
-      <c r="C71" s="3" t="n">
+      <c r="C71" t="n">
         <v>1</v>
       </c>
       <c r="D71" s="2" t="n">
@@ -1884,7 +3175,7 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="4" t="n">
+      <c r="A72" s="5" t="n">
         <v>45664</v>
       </c>
       <c r="B72" t="inlineStr">
@@ -1892,7 +3183,7 @@
           <t>Monitor</t>
         </is>
       </c>
-      <c r="C72" s="3" t="n">
+      <c r="C72" t="n">
         <v>9</v>
       </c>
       <c r="D72" s="2" t="n">
@@ -1903,7 +3194,7 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="4" t="n">
+      <c r="A73" s="5" t="n">
         <v>45665</v>
       </c>
       <c r="B73" t="inlineStr">
@@ -1911,7 +3202,7 @@
           <t>Notebook</t>
         </is>
       </c>
-      <c r="C73" s="3" t="n">
+      <c r="C73" t="n">
         <v>1</v>
       </c>
       <c r="D73" s="2" t="n">
@@ -1922,7 +3213,7 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="4" t="n">
+      <c r="A74" s="5" t="n">
         <v>45665</v>
       </c>
       <c r="B74" t="inlineStr">
@@ -1930,7 +3221,7 @@
           <t>HD</t>
         </is>
       </c>
-      <c r="C74" s="3" t="n">
+      <c r="C74" t="n">
         <v>4</v>
       </c>
       <c r="D74" s="2" t="n">
@@ -1941,7 +3232,7 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="4" t="n">
+      <c r="A75" s="5" t="n">
         <v>45667</v>
       </c>
       <c r="B75" t="inlineStr">
@@ -1949,7 +3240,7 @@
           <t>Impressora</t>
         </is>
       </c>
-      <c r="C75" s="3" t="n">
+      <c r="C75" t="n">
         <v>7</v>
       </c>
       <c r="D75" s="2" t="n">
@@ -1960,7 +3251,7 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="4" t="n">
+      <c r="A76" s="5" t="n">
         <v>45667</v>
       </c>
       <c r="B76" t="inlineStr">
@@ -1968,7 +3259,7 @@
           <t>SSD</t>
         </is>
       </c>
-      <c r="C76" s="3" t="n">
+      <c r="C76" t="n">
         <v>7</v>
       </c>
       <c r="D76" s="2" t="n">
@@ -1979,7 +3270,7 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="4" t="n">
+      <c r="A77" s="5" t="n">
         <v>45668</v>
       </c>
       <c r="B77" t="inlineStr">
@@ -1987,7 +3278,7 @@
           <t>HD</t>
         </is>
       </c>
-      <c r="C77" s="3" t="n">
+      <c r="C77" t="n">
         <v>7</v>
       </c>
       <c r="D77" s="2" t="n">
@@ -1998,7 +3289,7 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="4" t="n">
+      <c r="A78" s="5" t="n">
         <v>45668</v>
       </c>
       <c r="B78" t="inlineStr">
@@ -2006,7 +3297,7 @@
           <t>HD</t>
         </is>
       </c>
-      <c r="C78" s="3" t="n">
+      <c r="C78" t="n">
         <v>10</v>
       </c>
       <c r="D78" s="2" t="n">
@@ -2017,7 +3308,7 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="4" t="n">
+      <c r="A79" s="5" t="n">
         <v>45670</v>
       </c>
       <c r="B79" t="inlineStr">
@@ -2025,7 +3316,7 @@
           <t>Monitor</t>
         </is>
       </c>
-      <c r="C79" s="3" t="n">
+      <c r="C79" t="n">
         <v>9</v>
       </c>
       <c r="D79" s="2" t="n">
@@ -2036,7 +3327,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="4" t="n">
+      <c r="A80" s="5" t="n">
         <v>45671</v>
       </c>
       <c r="B80" t="inlineStr">
@@ -2044,7 +3335,7 @@
           <t>Webcam</t>
         </is>
       </c>
-      <c r="C80" s="3" t="n">
+      <c r="C80" t="n">
         <v>5</v>
       </c>
       <c r="D80" s="2" t="n">
@@ -2055,7 +3346,7 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="4" t="n">
+      <c r="A81" s="5" t="n">
         <v>45673</v>
       </c>
       <c r="B81" t="inlineStr">
@@ -2063,7 +3354,7 @@
           <t>Impressora</t>
         </is>
       </c>
-      <c r="C81" s="3" t="n">
+      <c r="C81" t="n">
         <v>4</v>
       </c>
       <c r="D81" s="2" t="n">
@@ -2074,7 +3365,7 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="4" t="n">
+      <c r="A82" s="5" t="n">
         <v>45673</v>
       </c>
       <c r="B82" t="inlineStr">
@@ -2082,7 +3373,7 @@
           <t>Notebook</t>
         </is>
       </c>
-      <c r="C82" s="3" t="n">
+      <c r="C82" t="n">
         <v>4</v>
       </c>
       <c r="D82" s="2" t="n">
@@ -2093,7 +3384,7 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="4" t="n">
+      <c r="A83" s="5" t="n">
         <v>45676</v>
       </c>
       <c r="B83" t="inlineStr">
@@ -2101,7 +3392,7 @@
           <t>SSD</t>
         </is>
       </c>
-      <c r="C83" s="3" t="n">
+      <c r="C83" t="n">
         <v>4</v>
       </c>
       <c r="D83" s="2" t="n">
@@ -2112,7 +3403,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="4" t="n">
+      <c r="A84" s="5" t="n">
         <v>45677</v>
       </c>
       <c r="B84" t="inlineStr">
@@ -2120,7 +3411,7 @@
           <t>HD</t>
         </is>
       </c>
-      <c r="C84" s="3" t="n">
+      <c r="C84" t="n">
         <v>6</v>
       </c>
       <c r="D84" s="2" t="n">
@@ -2131,7 +3422,7 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="4" t="n">
+      <c r="A85" s="5" t="n">
         <v>45678</v>
       </c>
       <c r="B85" t="inlineStr">
@@ -2139,7 +3430,7 @@
           <t>HD</t>
         </is>
       </c>
-      <c r="C85" s="3" t="n">
+      <c r="C85" t="n">
         <v>7</v>
       </c>
       <c r="D85" s="2" t="n">
@@ -2150,7 +3441,7 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="4" t="n">
+      <c r="A86" s="5" t="n">
         <v>45678</v>
       </c>
       <c r="B86" t="inlineStr">
@@ -2158,7 +3449,7 @@
           <t>Webcam</t>
         </is>
       </c>
-      <c r="C86" s="3" t="n">
+      <c r="C86" t="n">
         <v>1</v>
       </c>
       <c r="D86" s="2" t="n">
@@ -2169,7 +3460,7 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="4" t="n">
+      <c r="A87" s="5" t="n">
         <v>45678</v>
       </c>
       <c r="B87" t="inlineStr">
@@ -2177,7 +3468,7 @@
           <t>Headset</t>
         </is>
       </c>
-      <c r="C87" s="3" t="n">
+      <c r="C87" t="n">
         <v>8</v>
       </c>
       <c r="D87" s="2" t="n">
@@ -2188,7 +3479,7 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="4" t="n">
+      <c r="A88" s="5" t="n">
         <v>45679</v>
       </c>
       <c r="B88" t="inlineStr">
@@ -2196,7 +3487,7 @@
           <t>Notebook</t>
         </is>
       </c>
-      <c r="C88" s="3" t="n">
+      <c r="C88" t="n">
         <v>10</v>
       </c>
       <c r="D88" s="2" t="n">
@@ -2207,7 +3498,7 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="4" t="n">
+      <c r="A89" s="5" t="n">
         <v>45679</v>
       </c>
       <c r="B89" t="inlineStr">
@@ -2215,7 +3506,7 @@
           <t>Headset</t>
         </is>
       </c>
-      <c r="C89" s="3" t="n">
+      <c r="C89" t="n">
         <v>6</v>
       </c>
       <c r="D89" s="2" t="n">
@@ -2226,7 +3517,7 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="4" t="n">
+      <c r="A90" s="5" t="n">
         <v>45679</v>
       </c>
       <c r="B90" t="inlineStr">
@@ -2234,7 +3525,7 @@
           <t>Headset</t>
         </is>
       </c>
-      <c r="C90" s="3" t="n">
+      <c r="C90" t="n">
         <v>7</v>
       </c>
       <c r="D90" s="2" t="n">
@@ -2245,7 +3536,7 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="4" t="n">
+      <c r="A91" s="5" t="n">
         <v>45680</v>
       </c>
       <c r="B91" t="inlineStr">
@@ -2253,7 +3544,7 @@
           <t>HD</t>
         </is>
       </c>
-      <c r="C91" s="3" t="n">
+      <c r="C91" t="n">
         <v>4</v>
       </c>
       <c r="D91" s="2" t="n">
@@ -2264,7 +3555,7 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="4" t="n">
+      <c r="A92" s="5" t="n">
         <v>45681</v>
       </c>
       <c r="B92" t="inlineStr">
@@ -2272,7 +3563,7 @@
           <t>Webcam</t>
         </is>
       </c>
-      <c r="C92" s="3" t="n">
+      <c r="C92" t="n">
         <v>7</v>
       </c>
       <c r="D92" s="2" t="n">
@@ -2283,7 +3574,7 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="4" t="n">
+      <c r="A93" s="5" t="n">
         <v>45684</v>
       </c>
       <c r="B93" t="inlineStr">
@@ -2291,7 +3582,7 @@
           <t>Mouse</t>
         </is>
       </c>
-      <c r="C93" s="3" t="n">
+      <c r="C93" t="n">
         <v>5</v>
       </c>
       <c r="D93" s="2" t="n">
@@ -2302,7 +3593,7 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="4" t="n">
+      <c r="A94" s="5" t="n">
         <v>45685</v>
       </c>
       <c r="B94" t="inlineStr">
@@ -2310,7 +3601,7 @@
           <t>Teclado</t>
         </is>
       </c>
-      <c r="C94" s="3" t="n">
+      <c r="C94" t="n">
         <v>5</v>
       </c>
       <c r="D94" s="2" t="n">
@@ -2321,7 +3612,7 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="4" t="n">
+      <c r="A95" s="5" t="n">
         <v>45685</v>
       </c>
       <c r="B95" t="inlineStr">
@@ -2329,7 +3620,7 @@
           <t>Webcam</t>
         </is>
       </c>
-      <c r="C95" s="3" t="n">
+      <c r="C95" t="n">
         <v>3</v>
       </c>
       <c r="D95" s="2" t="n">
@@ -2340,7 +3631,7 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="4" t="n">
+      <c r="A96" s="5" t="n">
         <v>45686</v>
       </c>
       <c r="B96" t="inlineStr">
@@ -2348,7 +3639,7 @@
           <t>Notebook</t>
         </is>
       </c>
-      <c r="C96" s="3" t="n">
+      <c r="C96" t="n">
         <v>8</v>
       </c>
       <c r="D96" s="2" t="n">
@@ -2359,7 +3650,7 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="4" t="n">
+      <c r="A97" s="5" t="n">
         <v>45688</v>
       </c>
       <c r="B97" t="inlineStr">
@@ -2367,7 +3658,7 @@
           <t>Mouse</t>
         </is>
       </c>
-      <c r="C97" s="3" t="n">
+      <c r="C97" t="n">
         <v>5</v>
       </c>
       <c r="D97" s="2" t="n">
@@ -2378,7 +3669,7 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="4" t="n">
+      <c r="A98" s="5" t="n">
         <v>45688</v>
       </c>
       <c r="B98" t="inlineStr">
@@ -2386,7 +3677,7 @@
           <t>Mouse</t>
         </is>
       </c>
-      <c r="C98" s="3" t="n">
+      <c r="C98" t="n">
         <v>10</v>
       </c>
       <c r="D98" s="2" t="n">
@@ -2397,7 +3688,7 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="4" t="n">
+      <c r="A99" s="5" t="n">
         <v>45688</v>
       </c>
       <c r="B99" t="inlineStr">
@@ -2405,7 +3696,7 @@
           <t>Teclado</t>
         </is>
       </c>
-      <c r="C99" s="3" t="n">
+      <c r="C99" t="n">
         <v>5</v>
       </c>
       <c r="D99" s="2" t="n">
@@ -2416,7 +3707,7 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="4" t="n">
+      <c r="A100" s="5" t="n">
         <v>45689</v>
       </c>
       <c r="B100" t="inlineStr">
@@ -2424,7 +3715,7 @@
           <t>Mouse</t>
         </is>
       </c>
-      <c r="C100" s="3" t="n">
+      <c r="C100" t="n">
         <v>7</v>
       </c>
       <c r="D100" s="2" t="n">
@@ -2435,7 +3726,7 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="4" t="n">
+      <c r="A101" s="5" t="n">
         <v>45689</v>
       </c>
       <c r="B101" t="inlineStr">
@@ -2443,7 +3734,7 @@
           <t>Impressora</t>
         </is>
       </c>
-      <c r="C101" s="3" t="n">
+      <c r="C101" t="n">
         <v>4</v>
       </c>
       <c r="D101" s="2" t="n">
@@ -2454,7 +3745,7 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="4" t="n">
+      <c r="A102" s="5" t="n">
         <v>45691</v>
       </c>
       <c r="B102" t="inlineStr">
@@ -2462,7 +3753,7 @@
           <t>Teclado</t>
         </is>
       </c>
-      <c r="C102" s="3" t="n">
+      <c r="C102" t="n">
         <v>8</v>
       </c>
       <c r="D102" s="2" t="n">
@@ -2473,7 +3764,7 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="4" t="n">
+      <c r="A103" s="5" t="n">
         <v>45691</v>
       </c>
       <c r="B103" t="inlineStr">
@@ -2481,7 +3772,7 @@
           <t>Teclado</t>
         </is>
       </c>
-      <c r="C103" s="3" t="n">
+      <c r="C103" t="n">
         <v>1</v>
       </c>
       <c r="D103" s="2" t="n">
@@ -2492,7 +3783,7 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="4" t="n">
+      <c r="A104" s="5" t="n">
         <v>45692</v>
       </c>
       <c r="B104" t="inlineStr">
@@ -2500,7 +3791,7 @@
           <t>Notebook</t>
         </is>
       </c>
-      <c r="C104" s="3" t="n">
+      <c r="C104" t="n">
         <v>8</v>
       </c>
       <c r="D104" s="2" t="n">
@@ -2511,7 +3802,7 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="4" t="n">
+      <c r="A105" s="5" t="n">
         <v>45693</v>
       </c>
       <c r="B105" t="inlineStr">
@@ -2519,7 +3810,7 @@
           <t>Teclado</t>
         </is>
       </c>
-      <c r="C105" s="3" t="n">
+      <c r="C105" t="n">
         <v>9</v>
       </c>
       <c r="D105" s="2" t="n">
@@ -2530,7 +3821,7 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="4" t="n">
+      <c r="A106" s="5" t="n">
         <v>45694</v>
       </c>
       <c r="B106" t="inlineStr">
@@ -2538,7 +3829,7 @@
           <t>Mouse</t>
         </is>
       </c>
-      <c r="C106" s="3" t="n">
+      <c r="C106" t="n">
         <v>4</v>
       </c>
       <c r="D106" s="2" t="n">
@@ -2549,7 +3840,7 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="4" t="n">
+      <c r="A107" s="5" t="n">
         <v>45695</v>
       </c>
       <c r="B107" t="inlineStr">
@@ -2557,7 +3848,7 @@
           <t>Teclado</t>
         </is>
       </c>
-      <c r="C107" s="3" t="n">
+      <c r="C107" t="n">
         <v>10</v>
       </c>
       <c r="D107" s="2" t="n">
@@ -2568,7 +3859,7 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="4" t="n">
+      <c r="A108" s="5" t="n">
         <v>45696</v>
       </c>
       <c r="B108" t="inlineStr">
@@ -2576,7 +3867,7 @@
           <t>Mouse</t>
         </is>
       </c>
-      <c r="C108" s="3" t="n">
+      <c r="C108" t="n">
         <v>3</v>
       </c>
       <c r="D108" s="2" t="n">
@@ -2587,7 +3878,7 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="4" t="n">
+      <c r="A109" s="5" t="n">
         <v>45700</v>
       </c>
       <c r="B109" t="inlineStr">
@@ -2595,7 +3886,7 @@
           <t>Notebook</t>
         </is>
       </c>
-      <c r="C109" s="3" t="n">
+      <c r="C109" t="n">
         <v>5</v>
       </c>
       <c r="D109" s="2" t="n">
@@ -2606,7 +3897,7 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="4" t="n">
+      <c r="A110" s="5" t="n">
         <v>45701</v>
       </c>
       <c r="B110" t="inlineStr">
@@ -2614,7 +3905,7 @@
           <t>Monitor</t>
         </is>
       </c>
-      <c r="C110" s="3" t="n">
+      <c r="C110" t="n">
         <v>5</v>
       </c>
       <c r="D110" s="2" t="n">
@@ -2625,7 +3916,7 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="4" t="n">
+      <c r="A111" s="5" t="n">
         <v>45705</v>
       </c>
       <c r="B111" t="inlineStr">
@@ -2633,7 +3924,7 @@
           <t>Headset</t>
         </is>
       </c>
-      <c r="C111" s="3" t="n">
+      <c r="C111" t="n">
         <v>10</v>
       </c>
       <c r="D111" s="2" t="n">
@@ -2644,7 +3935,7 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="4" t="n">
+      <c r="A112" s="5" t="n">
         <v>45708</v>
       </c>
       <c r="B112" t="inlineStr">
@@ -2652,7 +3943,7 @@
           <t>Impressora</t>
         </is>
       </c>
-      <c r="C112" s="3" t="n">
+      <c r="C112" t="n">
         <v>8</v>
       </c>
       <c r="D112" s="2" t="n">
@@ -2663,7 +3954,7 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="4" t="n">
+      <c r="A113" s="5" t="n">
         <v>45708</v>
       </c>
       <c r="B113" t="inlineStr">
@@ -2671,7 +3962,7 @@
           <t>Headset</t>
         </is>
       </c>
-      <c r="C113" s="3" t="n">
+      <c r="C113" t="n">
         <v>7</v>
       </c>
       <c r="D113" s="2" t="n">
@@ -2682,7 +3973,7 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="4" t="n">
+      <c r="A114" s="5" t="n">
         <v>45710</v>
       </c>
       <c r="B114" t="inlineStr">
@@ -2690,7 +3981,7 @@
           <t>Impressora</t>
         </is>
       </c>
-      <c r="C114" s="3" t="n">
+      <c r="C114" t="n">
         <v>8</v>
       </c>
       <c r="D114" s="2" t="n">
@@ -2701,7 +3992,7 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="4" t="n">
+      <c r="A115" s="5" t="n">
         <v>45711</v>
       </c>
       <c r="B115" t="inlineStr">
@@ -2709,7 +4000,7 @@
           <t>Mouse</t>
         </is>
       </c>
-      <c r="C115" s="3" t="n">
+      <c r="C115" t="n">
         <v>3</v>
       </c>
       <c r="D115" s="2" t="n">
@@ -2720,7 +4011,7 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="4" t="n">
+      <c r="A116" s="5" t="n">
         <v>45711</v>
       </c>
       <c r="B116" t="inlineStr">
@@ -2728,7 +4019,7 @@
           <t>Monitor</t>
         </is>
       </c>
-      <c r="C116" s="3" t="n">
+      <c r="C116" t="n">
         <v>4</v>
       </c>
       <c r="D116" s="2" t="n">
@@ -2739,7 +4030,7 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="4" t="n">
+      <c r="A117" s="5" t="n">
         <v>45712</v>
       </c>
       <c r="B117" t="inlineStr">
@@ -2747,7 +4038,7 @@
           <t>Webcam</t>
         </is>
       </c>
-      <c r="C117" s="3" t="n">
+      <c r="C117" t="n">
         <v>2</v>
       </c>
       <c r="D117" s="2" t="n">
@@ -2758,7 +4049,7 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="4" t="n">
+      <c r="A118" s="5" t="n">
         <v>45712</v>
       </c>
       <c r="B118" t="inlineStr">
@@ -2766,7 +4057,7 @@
           <t>Headset</t>
         </is>
       </c>
-      <c r="C118" s="3" t="n">
+      <c r="C118" t="n">
         <v>4</v>
       </c>
       <c r="D118" s="2" t="n">
@@ -2777,7 +4068,7 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="4" t="n">
+      <c r="A119" s="5" t="n">
         <v>45715</v>
       </c>
       <c r="B119" t="inlineStr">
@@ -2785,7 +4076,7 @@
           <t>Headset</t>
         </is>
       </c>
-      <c r="C119" s="3" t="n">
+      <c r="C119" t="n">
         <v>10</v>
       </c>
       <c r="D119" s="2" t="n">
@@ -2796,7 +4087,7 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="4" t="n">
+      <c r="A120" s="5" t="n">
         <v>45715</v>
       </c>
       <c r="B120" t="inlineStr">
@@ -2804,7 +4095,7 @@
           <t>Monitor</t>
         </is>
       </c>
-      <c r="C120" s="3" t="n">
+      <c r="C120" t="n">
         <v>9</v>
       </c>
       <c r="D120" s="2" t="n">
@@ -2815,7 +4106,7 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="4" t="n">
+      <c r="A121" s="5" t="n">
         <v>45716</v>
       </c>
       <c r="B121" t="inlineStr">
@@ -2823,7 +4114,7 @@
           <t>SSD</t>
         </is>
       </c>
-      <c r="C121" s="3" t="n">
+      <c r="C121" t="n">
         <v>10</v>
       </c>
       <c r="D121" s="2" t="n">
@@ -2834,7 +4125,7 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="4" t="n">
+      <c r="A122" s="5" t="n">
         <v>45718</v>
       </c>
       <c r="B122" t="inlineStr">
@@ -2842,7 +4133,7 @@
           <t>Monitor</t>
         </is>
       </c>
-      <c r="C122" s="3" t="n">
+      <c r="C122" t="n">
         <v>7</v>
       </c>
       <c r="D122" s="2" t="n">
@@ -2853,7 +4144,7 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="4" t="n">
+      <c r="A123" s="5" t="n">
         <v>45718</v>
       </c>
       <c r="B123" t="inlineStr">
@@ -2861,7 +4152,7 @@
           <t>HD</t>
         </is>
       </c>
-      <c r="C123" s="3" t="n">
+      <c r="C123" t="n">
         <v>9</v>
       </c>
       <c r="D123" s="2" t="n">
@@ -2872,7 +4163,7 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="4" t="n">
+      <c r="A124" s="5" t="n">
         <v>45720</v>
       </c>
       <c r="B124" t="inlineStr">
@@ -2880,7 +4171,7 @@
           <t>HD</t>
         </is>
       </c>
-      <c r="C124" s="3" t="n">
+      <c r="C124" t="n">
         <v>3</v>
       </c>
       <c r="D124" s="2" t="n">
@@ -2891,7 +4182,7 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="4" t="n">
+      <c r="A125" s="5" t="n">
         <v>45722</v>
       </c>
       <c r="B125" t="inlineStr">
@@ -2899,7 +4190,7 @@
           <t>SSD</t>
         </is>
       </c>
-      <c r="C125" s="3" t="n">
+      <c r="C125" t="n">
         <v>3</v>
       </c>
       <c r="D125" s="2" t="n">
@@ -2910,7 +4201,7 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="4" t="n">
+      <c r="A126" s="5" t="n">
         <v>45722</v>
       </c>
       <c r="B126" t="inlineStr">
@@ -2918,7 +4209,7 @@
           <t>HD</t>
         </is>
       </c>
-      <c r="C126" s="3" t="n">
+      <c r="C126" t="n">
         <v>2</v>
       </c>
       <c r="D126" s="2" t="n">
@@ -2929,7 +4220,7 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="4" t="n">
+      <c r="A127" s="5" t="n">
         <v>45723</v>
       </c>
       <c r="B127" t="inlineStr">
@@ -2937,7 +4228,7 @@
           <t>Teclado</t>
         </is>
       </c>
-      <c r="C127" s="3" t="n">
+      <c r="C127" t="n">
         <v>5</v>
       </c>
       <c r="D127" s="2" t="n">
@@ -2948,7 +4239,7 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="4" t="n">
+      <c r="A128" s="5" t="n">
         <v>45725</v>
       </c>
       <c r="B128" t="inlineStr">
@@ -2956,7 +4247,7 @@
           <t>Impressora</t>
         </is>
       </c>
-      <c r="C128" s="3" t="n">
+      <c r="C128" t="n">
         <v>7</v>
       </c>
       <c r="D128" s="2" t="n">
@@ -2967,7 +4258,7 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="4" t="n">
+      <c r="A129" s="5" t="n">
         <v>45726</v>
       </c>
       <c r="B129" t="inlineStr">
@@ -2975,7 +4266,7 @@
           <t>SSD</t>
         </is>
       </c>
-      <c r="C129" s="3" t="n">
+      <c r="C129" t="n">
         <v>6</v>
       </c>
       <c r="D129" s="2" t="n">
@@ -2986,7 +4277,7 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="4" t="n">
+      <c r="A130" s="5" t="n">
         <v>45726</v>
       </c>
       <c r="B130" t="inlineStr">
@@ -2994,7 +4285,7 @@
           <t>Notebook</t>
         </is>
       </c>
-      <c r="C130" s="3" t="n">
+      <c r="C130" t="n">
         <v>4</v>
       </c>
       <c r="D130" s="2" t="n">
@@ -3005,7 +4296,7 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="4" t="n">
+      <c r="A131" s="5" t="n">
         <v>45727</v>
       </c>
       <c r="B131" t="inlineStr">
@@ -3013,7 +4304,7 @@
           <t>Monitor</t>
         </is>
       </c>
-      <c r="C131" s="3" t="n">
+      <c r="C131" t="n">
         <v>10</v>
       </c>
       <c r="D131" s="2" t="n">
@@ -3024,7 +4315,7 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="4" t="n">
+      <c r="A132" s="5" t="n">
         <v>45728</v>
       </c>
       <c r="B132" t="inlineStr">
@@ -3032,7 +4323,7 @@
           <t>Webcam</t>
         </is>
       </c>
-      <c r="C132" s="3" t="n">
+      <c r="C132" t="n">
         <v>6</v>
       </c>
       <c r="D132" s="2" t="n">
@@ -3043,7 +4334,7 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="4" t="n">
+      <c r="A133" s="5" t="n">
         <v>45730</v>
       </c>
       <c r="B133" t="inlineStr">
@@ -3051,7 +4342,7 @@
           <t>Mouse</t>
         </is>
       </c>
-      <c r="C133" s="3" t="n">
+      <c r="C133" t="n">
         <v>9</v>
       </c>
       <c r="D133" s="2" t="n">
@@ -3062,7 +4353,7 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="4" t="n">
+      <c r="A134" s="5" t="n">
         <v>45731</v>
       </c>
       <c r="B134" t="inlineStr">
@@ -3070,7 +4361,7 @@
           <t>SSD</t>
         </is>
       </c>
-      <c r="C134" s="3" t="n">
+      <c r="C134" t="n">
         <v>9</v>
       </c>
       <c r="D134" s="2" t="n">
@@ -3081,7 +4372,7 @@
       </c>
     </row>
     <row r="135">
-      <c r="A135" s="4" t="n">
+      <c r="A135" s="5" t="n">
         <v>45733</v>
       </c>
       <c r="B135" t="inlineStr">
@@ -3089,7 +4380,7 @@
           <t>HD</t>
         </is>
       </c>
-      <c r="C135" s="3" t="n">
+      <c r="C135" t="n">
         <v>6</v>
       </c>
       <c r="D135" s="2" t="n">
@@ -3100,7 +4391,7 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="4" t="n">
+      <c r="A136" s="5" t="n">
         <v>45735</v>
       </c>
       <c r="B136" t="inlineStr">
@@ -3108,7 +4399,7 @@
           <t>Headset</t>
         </is>
       </c>
-      <c r="C136" s="3" t="n">
+      <c r="C136" t="n">
         <v>6</v>
       </c>
       <c r="D136" s="2" t="n">
@@ -3119,7 +4410,7 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" s="4" t="n">
+      <c r="A137" s="5" t="n">
         <v>45735</v>
       </c>
       <c r="B137" t="inlineStr">
@@ -3127,7 +4418,7 @@
           <t>SSD</t>
         </is>
       </c>
-      <c r="C137" s="3" t="n">
+      <c r="C137" t="n">
         <v>6</v>
       </c>
       <c r="D137" s="2" t="n">
@@ -3138,7 +4429,7 @@
       </c>
     </row>
     <row r="138">
-      <c r="A138" s="4" t="n">
+      <c r="A138" s="5" t="n">
         <v>45737</v>
       </c>
       <c r="B138" t="inlineStr">
@@ -3146,7 +4437,7 @@
           <t>HD</t>
         </is>
       </c>
-      <c r="C138" s="3" t="n">
+      <c r="C138" t="n">
         <v>2</v>
       </c>
       <c r="D138" s="2" t="n">
@@ -3157,7 +4448,7 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="4" t="n">
+      <c r="A139" s="5" t="n">
         <v>45737</v>
       </c>
       <c r="B139" t="inlineStr">
@@ -3165,7 +4456,7 @@
           <t>Teclado</t>
         </is>
       </c>
-      <c r="C139" s="3" t="n">
+      <c r="C139" t="n">
         <v>1</v>
       </c>
       <c r="D139" s="2" t="n">
@@ -3176,7 +4467,7 @@
       </c>
     </row>
     <row r="140">
-      <c r="A140" s="4" t="n">
+      <c r="A140" s="5" t="n">
         <v>45737</v>
       </c>
       <c r="B140" t="inlineStr">
@@ -3184,7 +4475,7 @@
           <t>Webcam</t>
         </is>
       </c>
-      <c r="C140" s="3" t="n">
+      <c r="C140" t="n">
         <v>3</v>
       </c>
       <c r="D140" s="2" t="n">
@@ -3195,7 +4486,7 @@
       </c>
     </row>
     <row r="141">
-      <c r="A141" s="4" t="n">
+      <c r="A141" s="5" t="n">
         <v>45738</v>
       </c>
       <c r="B141" t="inlineStr">
@@ -3203,7 +4494,7 @@
           <t>Teclado</t>
         </is>
       </c>
-      <c r="C141" s="3" t="n">
+      <c r="C141" t="n">
         <v>7</v>
       </c>
       <c r="D141" s="2" t="n">
@@ -3214,7 +4505,7 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" s="4" t="n">
+      <c r="A142" s="5" t="n">
         <v>45739</v>
       </c>
       <c r="B142" t="inlineStr">
@@ -3222,7 +4513,7 @@
           <t>Monitor</t>
         </is>
       </c>
-      <c r="C142" s="3" t="n">
+      <c r="C142" t="n">
         <v>10</v>
       </c>
       <c r="D142" s="2" t="n">
@@ -3233,7 +4524,7 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="4" t="n">
+      <c r="A143" s="5" t="n">
         <v>45739</v>
       </c>
       <c r="B143" t="inlineStr">
@@ -3241,7 +4532,7 @@
           <t>Monitor</t>
         </is>
       </c>
-      <c r="C143" s="3" t="n">
+      <c r="C143" t="n">
         <v>9</v>
       </c>
       <c r="D143" s="2" t="n">
@@ -3252,7 +4543,7 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" s="4" t="n">
+      <c r="A144" s="5" t="n">
         <v>45743</v>
       </c>
       <c r="B144" t="inlineStr">
@@ -3260,7 +4551,7 @@
           <t>Monitor</t>
         </is>
       </c>
-      <c r="C144" s="3" t="n">
+      <c r="C144" t="n">
         <v>5</v>
       </c>
       <c r="D144" s="2" t="n">
@@ -3271,7 +4562,7 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="4" t="n">
+      <c r="A145" s="5" t="n">
         <v>45743</v>
       </c>
       <c r="B145" t="inlineStr">
@@ -3279,7 +4570,7 @@
           <t>Notebook</t>
         </is>
       </c>
-      <c r="C145" s="3" t="n">
+      <c r="C145" t="n">
         <v>6</v>
       </c>
       <c r="D145" s="2" t="n">
@@ -3290,7 +4581,7 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" s="4" t="n">
+      <c r="A146" s="5" t="n">
         <v>45744</v>
       </c>
       <c r="B146" t="inlineStr">
@@ -3298,7 +4589,7 @@
           <t>Monitor</t>
         </is>
       </c>
-      <c r="C146" s="3" t="n">
+      <c r="C146" t="n">
         <v>4</v>
       </c>
       <c r="D146" s="2" t="n">
@@ -3309,7 +4600,7 @@
       </c>
     </row>
     <row r="147">
-      <c r="A147" s="4" t="n">
+      <c r="A147" s="5" t="n">
         <v>45744</v>
       </c>
       <c r="B147" t="inlineStr">
@@ -3317,7 +4608,7 @@
           <t>SSD</t>
         </is>
       </c>
-      <c r="C147" s="3" t="n">
+      <c r="C147" t="n">
         <v>1</v>
       </c>
       <c r="D147" s="2" t="n">
@@ -3328,7 +4619,7 @@
       </c>
     </row>
     <row r="148">
-      <c r="A148" s="4" t="n">
+      <c r="A148" s="5" t="n">
         <v>45744</v>
       </c>
       <c r="B148" t="inlineStr">
@@ -3336,7 +4627,7 @@
           <t>Headset</t>
         </is>
       </c>
-      <c r="C148" s="3" t="n">
+      <c r="C148" t="n">
         <v>4</v>
       </c>
       <c r="D148" s="2" t="n">
@@ -3347,7 +4638,7 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" s="4" t="n">
+      <c r="A149" s="5" t="n">
         <v>45744</v>
       </c>
       <c r="B149" t="inlineStr">
@@ -3355,7 +4646,7 @@
           <t>Webcam</t>
         </is>
       </c>
-      <c r="C149" s="3" t="n">
+      <c r="C149" t="n">
         <v>8</v>
       </c>
       <c r="D149" s="2" t="n">
@@ -3366,7 +4657,7 @@
       </c>
     </row>
     <row r="150">
-      <c r="A150" s="4" t="n">
+      <c r="A150" s="5" t="n">
         <v>45746</v>
       </c>
       <c r="B150" t="inlineStr">
@@ -3374,7 +4665,7 @@
           <t>Mouse</t>
         </is>
       </c>
-      <c r="C150" s="3" t="n">
+      <c r="C150" t="n">
         <v>10</v>
       </c>
       <c r="D150" s="2" t="n">
@@ -3385,7 +4676,7 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" s="4" t="n">
+      <c r="A151" s="5" t="n">
         <v>45746</v>
       </c>
       <c r="B151" t="inlineStr">
@@ -3393,7 +4684,7 @@
           <t>SSD</t>
         </is>
       </c>
-      <c r="C151" s="3" t="n">
+      <c r="C151" t="n">
         <v>5</v>
       </c>
       <c r="D151" s="2" t="n">

</xml_diff>